<commit_message>
xóa file vs để check lỗi
</commit_message>
<xml_diff>
--- a/aspnet.xlsx
+++ b/aspnet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kimhu\Desktop\RapChieuPhim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D50386-DC3B-4CAB-9D4C-A55EE6E71E0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D90977AE-A1E1-489F-9F2B-AC8F8E2D2D16}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>STT</t>
   </si>
@@ -97,9 +97,6 @@
   </si>
   <si>
     <t>Hoàng</t>
-  </si>
-  <si>
-    <t>*</t>
   </si>
   <si>
     <t>*socket.io</t>
@@ -730,8 +727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -877,8 +874,8 @@
       <c r="D9" s="12">
         <v>0.5</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>21</v>
+      <c r="E9" s="1">
+        <v>0.5</v>
       </c>
       <c r="F9" s="19"/>
       <c r="G9" s="19"/>
@@ -941,7 +938,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F13" s="19"/>
       <c r="G13" s="19"/>
@@ -971,6 +968,9 @@
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="E15" s="1">
         <v>0.5</v>
       </c>
       <c r="F15" s="19"/>

</xml_diff>

<commit_message>
Thêm xong nút tìm kiếm , và hoàn thành chức năng tìm kiếm với tên đăng nhập trong bảng tài khoản
</commit_message>
<xml_diff>
--- a/aspnet.xlsx
+++ b/aspnet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kimhu\Desktop\RapChieuPhim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D90977AE-A1E1-489F-9F2B-AC8F8E2D2D16}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4A3B3DC-9EB0-4D0B-802C-80F5B0367182}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -728,7 +728,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
tạo xong form đăng nhập admin, và sử lý xong trạng thái đăng nhập
</commit_message>
<xml_diff>
--- a/aspnet.xlsx
+++ b/aspnet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kimhu\Desktop\RapChieuPhim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4A3B3DC-9EB0-4D0B-802C-80F5B0367182}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7D2AD09-3E3D-4A20-BFDA-6F933F395128}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -727,8 +727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -970,9 +970,6 @@
       <c r="D15" s="12">
         <v>0.5</v>
       </c>
-      <c r="E15" s="1">
-        <v>0.5</v>
-      </c>
       <c r="F15" s="19"/>
       <c r="G15" s="19"/>
       <c r="H15" s="19"/>

</xml_diff>

<commit_message>
sử lý xong session đăng nhập tài khoản
</commit_message>
<xml_diff>
--- a/aspnet.xlsx
+++ b/aspnet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kimhu\Desktop\RapChieuPhim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7D2AD09-3E3D-4A20-BFDA-6F933F395128}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F56FC274-95C0-4F84-9AF4-EF10FB99FD9C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -728,7 +728,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -811,6 +811,9 @@
       <c r="D5" s="12">
         <v>1</v>
       </c>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
       <c r="F5" s="19"/>
       <c r="G5" s="19"/>
       <c r="H5" s="19"/>
@@ -824,6 +827,9 @@
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="12">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1">
         <v>1</v>
       </c>
       <c r="F6" s="19"/>

</xml_diff>